<commit_message>
add emsl id in dilution sheet
</commit_message>
<xml_diff>
--- a/SPE/24-04-12_TEMPEST_IS_sample_prep.xlsx
+++ b/SPE/24-04-12_TEMPEST_IS_sample_prep.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/jieun_kim_pnnl_gov/Documents/Desktop/COMPASS/TEMPEST/ionic strength exp/24-04-09_Ionic strength exp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimj704/Github/tempest_ionic_strength/SPE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="579" documentId="8_{7356F863-DDFE-C24B-85DE-156BEB0C1AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C244A55-2A10-0F47-87AA-9042308D6CCE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2D0A3B-D890-8149-9A24-CD274D5809F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="1500" windowWidth="38400" windowHeight="19400" xr2:uid="{D8F0235E-A0B3-244A-A783-4CC003662F90}"/>
+    <workbookView xWindow="7240" yWindow="3120" windowWidth="14400" windowHeight="9660" activeTab="1" xr2:uid="{D8F0235E-A0B3-244A-A783-4CC003662F90}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="149">
   <si>
     <t>Random_ID</t>
   </si>
@@ -480,6 +481,9 @@
   </si>
   <si>
     <t>Estimated sample (g)</t>
+  </si>
+  <si>
+    <t>Actual_Vol_SPEd_ml</t>
   </si>
 </sst>
 </file>
@@ -487,7 +491,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -621,10 +625,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,10 +644,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -968,8 +968,8 @@
   </sheetPr>
   <dimension ref="A1:X134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H124" sqref="H124"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1169,14 +1169,14 @@
         <v>26.3749</v>
       </c>
       <c r="L9" s="16">
-        <f t="shared" ref="L7:L70" si="2">E9-K9</f>
+        <f t="shared" ref="L9:L69" si="2">E9-K9</f>
         <v>11.027800000000003</v>
       </c>
       <c r="N9" s="16">
         <v>7.8788999999999998</v>
       </c>
       <c r="O9" s="16">
-        <f t="shared" ref="O7:O70" si="3">N9-I9</f>
+        <f t="shared" ref="O9:O69" si="3">N9-I9</f>
         <v>0.44519999999999982</v>
       </c>
       <c r="P9" s="18">
@@ -1226,7 +1226,7 @@
         <v>0.42269999999999985</v>
       </c>
       <c r="P10" s="18">
-        <f t="shared" ref="P7:P70" si="4">(O10/$X$9)*1000</f>
+        <f t="shared" ref="P10:P69" si="4">(O10/$X$9)*1000</f>
         <v>0.53371212121212108</v>
       </c>
     </row>
@@ -3395,18 +3395,18 @@
         <v>26.3475</v>
       </c>
       <c r="L72">
-        <f t="shared" ref="L71:L131" si="7">E72-K72</f>
+        <f t="shared" ref="L72:L131" si="7">E72-K72</f>
         <v>13.137499999999999</v>
       </c>
       <c r="N72">
         <v>8.1189999999999998</v>
       </c>
       <c r="O72">
-        <f t="shared" ref="O71:O131" si="8">N72-I72</f>
+        <f t="shared" ref="O72:O131" si="8">N72-I72</f>
         <v>0.68140000000000001</v>
       </c>
       <c r="P72" s="15">
-        <f t="shared" ref="P71:P131" si="9">(O72/$X$9)*1000</f>
+        <f t="shared" ref="P72:P131" si="9">(O72/$X$9)*1000</f>
         <v>0.86035353535353543</v>
       </c>
     </row>
@@ -5494,4 +5494,1170 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="36" fitToHeight="2" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F039119E-70A9-DE49-AEE2-52C3D73CEF2E}">
+  <dimension ref="A1:B115"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>Sheet1!A6</f>
+        <v>TMP_IS_1_A</v>
+      </c>
+      <c r="B2">
+        <f>Sheet1!L6</f>
+        <v>9.7325999999999979</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f>Sheet1!A9</f>
+        <v>TMP_IS_2_A</v>
+      </c>
+      <c r="B3">
+        <f>Sheet1!L9</f>
+        <v>11.027800000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="str">
+        <f>Sheet1!A10</f>
+        <v>TMP_IS_2_B</v>
+      </c>
+      <c r="B4">
+        <f>Sheet1!L10</f>
+        <v>12.514199999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="str">
+        <f>Sheet1!A11</f>
+        <v>TMP_IS_2_C</v>
+      </c>
+      <c r="B5">
+        <f>Sheet1!L11</f>
+        <v>13.372999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="str">
+        <f>Sheet1!A12</f>
+        <v>TMP_IS_3_A</v>
+      </c>
+      <c r="B6">
+        <f>Sheet1!L12</f>
+        <v>15.910099999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="str">
+        <f>Sheet1!A13</f>
+        <v>TMP_IS_3_B</v>
+      </c>
+      <c r="B7">
+        <f>Sheet1!L13</f>
+        <v>16.421500000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="str">
+        <f>Sheet1!A14</f>
+        <v>TMP_IS_3_C</v>
+      </c>
+      <c r="B8">
+        <f>Sheet1!L14</f>
+        <v>14.998900000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="str">
+        <f>Sheet1!A15</f>
+        <v>TMP_IS_4_A</v>
+      </c>
+      <c r="B9">
+        <f>Sheet1!L15</f>
+        <v>14.9177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="str">
+        <f>Sheet1!A16</f>
+        <v>TMP_IS_4_B</v>
+      </c>
+      <c r="B10">
+        <f>Sheet1!L16</f>
+        <v>16.1069</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="str">
+        <f>Sheet1!A17</f>
+        <v>TMP_IS_4_C</v>
+      </c>
+      <c r="B11">
+        <f>Sheet1!L17</f>
+        <v>15.8428</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="str">
+        <f>Sheet1!A18</f>
+        <v>TMP_IS_5_A</v>
+      </c>
+      <c r="B12">
+        <f>Sheet1!L18</f>
+        <v>17.210500000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="str">
+        <f>Sheet1!A19</f>
+        <v>TMP_IS_5_B</v>
+      </c>
+      <c r="B13">
+        <f>Sheet1!L19</f>
+        <v>14.848200000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="str">
+        <f>Sheet1!A20</f>
+        <v>TMP_IS_5_C</v>
+      </c>
+      <c r="B14">
+        <f>Sheet1!L20</f>
+        <v>15.162699999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="str">
+        <f>Sheet1!A21</f>
+        <v>TMP_IS_6_A</v>
+      </c>
+      <c r="B15">
+        <f>Sheet1!L21</f>
+        <v>15.639900000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="str">
+        <f>Sheet1!A22</f>
+        <v>TMP_IS_6_B</v>
+      </c>
+      <c r="B16">
+        <f>Sheet1!L22</f>
+        <v>15.935000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="str">
+        <f>Sheet1!A23</f>
+        <v>TMP_IS_6_C</v>
+      </c>
+      <c r="B17">
+        <f>Sheet1!L23</f>
+        <v>15.1158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="str">
+        <f>Sheet1!A24</f>
+        <v>TMP_IS_7_A</v>
+      </c>
+      <c r="B18">
+        <f>Sheet1!L24</f>
+        <v>15.773099999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="str">
+        <f>Sheet1!A25</f>
+        <v>TMP_IS_7_B</v>
+      </c>
+      <c r="B19">
+        <f>Sheet1!L25</f>
+        <v>15.735500000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="str">
+        <f>Sheet1!A26</f>
+        <v>TMP_IS_7_C</v>
+      </c>
+      <c r="B20">
+        <f>Sheet1!L26</f>
+        <v>15.271100000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="str">
+        <f>Sheet1!A27</f>
+        <v>TMP_IS_8_A</v>
+      </c>
+      <c r="B21">
+        <f>Sheet1!L27</f>
+        <v>6.9171000000000014</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="str">
+        <f>Sheet1!A30</f>
+        <v>TMP_IS_9_A</v>
+      </c>
+      <c r="B22">
+        <f>Sheet1!L30</f>
+        <v>14.482499999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="str">
+        <f>Sheet1!A31</f>
+        <v>TMP_IS_9_B</v>
+      </c>
+      <c r="B23">
+        <f>Sheet1!L31</f>
+        <v>13.730499999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="str">
+        <f>Sheet1!A32</f>
+        <v>TMP_IS_9_C</v>
+      </c>
+      <c r="B24">
+        <f>Sheet1!L32</f>
+        <v>15.085300000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="str">
+        <f>Sheet1!A33</f>
+        <v>TMP_IS_10_A</v>
+      </c>
+      <c r="B25">
+        <f>Sheet1!L33</f>
+        <v>14.227200000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="str">
+        <f>Sheet1!A34</f>
+        <v>TMP_IS_10_B</v>
+      </c>
+      <c r="B26">
+        <f>Sheet1!L34</f>
+        <v>14.733000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="str">
+        <f>Sheet1!A35</f>
+        <v>TMP_IS_10_C</v>
+      </c>
+      <c r="B27">
+        <f>Sheet1!L35</f>
+        <v>14.936800000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="str">
+        <f>Sheet1!A36</f>
+        <v>TMP_IS_11_A</v>
+      </c>
+      <c r="B28">
+        <f>Sheet1!L36</f>
+        <v>15.149700000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="str">
+        <f>Sheet1!A37</f>
+        <v>TMP_IS_11_B</v>
+      </c>
+      <c r="B29">
+        <f>Sheet1!L37</f>
+        <v>15.426000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="str">
+        <f>Sheet1!A38</f>
+        <v>TMP_IS_11_C</v>
+      </c>
+      <c r="B30">
+        <f>Sheet1!L38</f>
+        <v>15.313599999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="str">
+        <f>Sheet1!A39</f>
+        <v>TMP_IS_12_A</v>
+      </c>
+      <c r="B31">
+        <f>Sheet1!L39</f>
+        <v>14.702899999999996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="str">
+        <f>Sheet1!A40</f>
+        <v>TMP_IS_12_B</v>
+      </c>
+      <c r="B32">
+        <f>Sheet1!L40</f>
+        <v>15.911000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="str">
+        <f>Sheet1!A41</f>
+        <v>TMP_IS_12_C</v>
+      </c>
+      <c r="B33">
+        <f>Sheet1!L41</f>
+        <v>14.867799999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="str">
+        <f>Sheet1!A42</f>
+        <v>TMP_IS_13_A</v>
+      </c>
+      <c r="B34">
+        <f>Sheet1!L42</f>
+        <v>16.507899999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="str">
+        <f>Sheet1!A43</f>
+        <v>TMP_IS_13_B</v>
+      </c>
+      <c r="B35">
+        <f>Sheet1!L43</f>
+        <v>15.423500000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="str">
+        <f>Sheet1!A44</f>
+        <v>TMP_IS_13_C</v>
+      </c>
+      <c r="B36">
+        <f>Sheet1!L44</f>
+        <v>16.476799999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="str">
+        <f>Sheet1!A45</f>
+        <v>TMP_IS_14_A</v>
+      </c>
+      <c r="B37">
+        <f>Sheet1!L45</f>
+        <v>15.654999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="str">
+        <f>Sheet1!A46</f>
+        <v>TMP_IS_14_B</v>
+      </c>
+      <c r="B38">
+        <f>Sheet1!L46</f>
+        <v>15.531200000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="str">
+        <f>Sheet1!A47</f>
+        <v>TMP_IS_14_C</v>
+      </c>
+      <c r="B39">
+        <f>Sheet1!L47</f>
+        <v>15.8398</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="str">
+        <f>Sheet1!A48</f>
+        <v>TMP_IS_15_A</v>
+      </c>
+      <c r="B40">
+        <f>Sheet1!L48</f>
+        <v>5.2635000000000005</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="str">
+        <f>Sheet1!A51</f>
+        <v>TMP_IS_16_A</v>
+      </c>
+      <c r="B41">
+        <f>Sheet1!L51</f>
+        <v>14.536999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="str">
+        <f>Sheet1!A52</f>
+        <v>TMP_IS_16_B</v>
+      </c>
+      <c r="B42">
+        <f>Sheet1!L52</f>
+        <v>15.285899999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="str">
+        <f>Sheet1!A53</f>
+        <v>TMP_IS_16_C</v>
+      </c>
+      <c r="B43">
+        <f>Sheet1!L53</f>
+        <v>14.509999999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="str">
+        <f>Sheet1!A54</f>
+        <v>TMP_IS_17_A</v>
+      </c>
+      <c r="B44">
+        <f>Sheet1!L54</f>
+        <v>15.662600000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="str">
+        <f>Sheet1!A55</f>
+        <v>TMP_IS_17_B</v>
+      </c>
+      <c r="B45">
+        <f>Sheet1!L55</f>
+        <v>15.876799999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="str">
+        <f>Sheet1!A56</f>
+        <v>TMP_IS_17_C</v>
+      </c>
+      <c r="B46">
+        <f>Sheet1!L56</f>
+        <v>15.810500000000005</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="str">
+        <f>Sheet1!A57</f>
+        <v>TMP_IS_18_A</v>
+      </c>
+      <c r="B47">
+        <f>Sheet1!L57</f>
+        <v>15.494799999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="str">
+        <f>Sheet1!A58</f>
+        <v>TMP_IS_18_B</v>
+      </c>
+      <c r="B48">
+        <f>Sheet1!L58</f>
+        <v>14.960499999999996</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="str">
+        <f>Sheet1!A59</f>
+        <v>TMP_IS_18_C</v>
+      </c>
+      <c r="B49">
+        <f>Sheet1!L59</f>
+        <v>15.409400000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="str">
+        <f>Sheet1!A60</f>
+        <v>TMP_IS_19_A</v>
+      </c>
+      <c r="B50">
+        <f>Sheet1!L60</f>
+        <v>14.695999999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="str">
+        <f>Sheet1!A61</f>
+        <v>TMP_IS_19_B</v>
+      </c>
+      <c r="B51">
+        <f>Sheet1!L61</f>
+        <v>14.891899999999996</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="str">
+        <f>Sheet1!A62</f>
+        <v>TMP_IS_19_C</v>
+      </c>
+      <c r="B52">
+        <f>Sheet1!L62</f>
+        <v>13.701499999999996</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="str">
+        <f>Sheet1!A63</f>
+        <v>TMP_IS_20_A</v>
+      </c>
+      <c r="B53">
+        <f>Sheet1!L63</f>
+        <v>14.862500000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="str">
+        <f>Sheet1!A64</f>
+        <v>TMP_IS_20_B</v>
+      </c>
+      <c r="B54">
+        <f>Sheet1!L64</f>
+        <v>14.709500000000002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="str">
+        <f>Sheet1!A65</f>
+        <v>TMP_IS_20_C</v>
+      </c>
+      <c r="B55">
+        <f>Sheet1!L65</f>
+        <v>15.510600000000004</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="str">
+        <f>Sheet1!A66</f>
+        <v>TMP_IS_21_A</v>
+      </c>
+      <c r="B56">
+        <f>Sheet1!L66</f>
+        <v>12.039400000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="str">
+        <f>Sheet1!A67</f>
+        <v>TMP_IS_21_B</v>
+      </c>
+      <c r="B57">
+        <f>Sheet1!L67</f>
+        <v>12.227699999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="str">
+        <f>Sheet1!A68</f>
+        <v>TMP_IS_21_C</v>
+      </c>
+      <c r="B58">
+        <f>Sheet1!L68</f>
+        <v>13.518400000000003</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="str">
+        <f>Sheet1!A69</f>
+        <v>TMP_IS_22_A</v>
+      </c>
+      <c r="B59">
+        <f>Sheet1!L69</f>
+        <v>9.8706000000000031</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="str">
+        <f>Sheet1!A72</f>
+        <v>TMP_IS_23_A</v>
+      </c>
+      <c r="B60">
+        <f>Sheet1!L72</f>
+        <v>13.137499999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="str">
+        <f>Sheet1!A73</f>
+        <v>TMP_IS_23_B</v>
+      </c>
+      <c r="B61">
+        <f>Sheet1!L73</f>
+        <v>14.143599999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="str">
+        <f>Sheet1!A74</f>
+        <v>TMP_IS_23_C</v>
+      </c>
+      <c r="B62">
+        <f>Sheet1!L74</f>
+        <v>13.355099999999997</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="str">
+        <f>Sheet1!A75</f>
+        <v>TMP_IS_24_A</v>
+      </c>
+      <c r="B63">
+        <f>Sheet1!L75</f>
+        <v>14.546700000000001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="str">
+        <f>Sheet1!A76</f>
+        <v>TMP_IS_24_B</v>
+      </c>
+      <c r="B64">
+        <f>Sheet1!L76</f>
+        <v>14.032600000000002</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="str">
+        <f>Sheet1!A77</f>
+        <v>TMP_IS_24_C</v>
+      </c>
+      <c r="B65">
+        <f>Sheet1!L77</f>
+        <v>13.772600000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="str">
+        <f>Sheet1!A78</f>
+        <v>TMP_IS_25_A</v>
+      </c>
+      <c r="B66">
+        <f>Sheet1!L78</f>
+        <v>12.7865</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="str">
+        <f>Sheet1!A79</f>
+        <v>TMP_IS_25_B</v>
+      </c>
+      <c r="B67">
+        <f>Sheet1!L79</f>
+        <v>14.584599999999998</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="str">
+        <f>Sheet1!A80</f>
+        <v>TMP_IS_25_C</v>
+      </c>
+      <c r="B68">
+        <f>Sheet1!L80</f>
+        <v>14.005400000000002</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="str">
+        <f>Sheet1!A81</f>
+        <v>TMP_IS_26_A</v>
+      </c>
+      <c r="B69">
+        <f>Sheet1!L81</f>
+        <v>13.924799999999998</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="str">
+        <f>Sheet1!A82</f>
+        <v>TMP_IS_26_B</v>
+      </c>
+      <c r="B70">
+        <f>Sheet1!L82</f>
+        <v>13.545299999999997</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="str">
+        <f>Sheet1!A83</f>
+        <v>TMP_IS_26_C</v>
+      </c>
+      <c r="B71">
+        <f>Sheet1!L83</f>
+        <v>12.870000000000005</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="str">
+        <f>Sheet1!A84</f>
+        <v>TMP_IS_27_A</v>
+      </c>
+      <c r="B72">
+        <f>Sheet1!L84</f>
+        <v>13.558000000000003</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="str">
+        <f>Sheet1!A85</f>
+        <v>TMP_IS_27_B</v>
+      </c>
+      <c r="B73">
+        <f>Sheet1!L85</f>
+        <v>14.2819</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="str">
+        <f>Sheet1!A86</f>
+        <v>TMP_IS_27_C</v>
+      </c>
+      <c r="B74">
+        <f>Sheet1!L86</f>
+        <v>14.288599999999995</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="str">
+        <f>Sheet1!A87</f>
+        <v>TMP_IS_28_A</v>
+      </c>
+      <c r="B75">
+        <f>Sheet1!L87</f>
+        <v>13.444500000000001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" t="str">
+        <f>Sheet1!A88</f>
+        <v>TMP_IS_28_B</v>
+      </c>
+      <c r="B76">
+        <f>Sheet1!L88</f>
+        <v>14.567899999999998</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" t="str">
+        <f>Sheet1!A89</f>
+        <v>TMP_IS_28_C</v>
+      </c>
+      <c r="B77">
+        <f>Sheet1!L89</f>
+        <v>14.155400000000004</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" t="str">
+        <f>Sheet1!A90</f>
+        <v>TMP_IS_29_A</v>
+      </c>
+      <c r="B78">
+        <f>Sheet1!L90</f>
+        <v>6.5828000000000024</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="str">
+        <f>Sheet1!A93</f>
+        <v>TMP_IS_30_A</v>
+      </c>
+      <c r="B79">
+        <f>Sheet1!L93</f>
+        <v>13.288399999999996</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="str">
+        <f>Sheet1!A94</f>
+        <v>TMP_IS_30_B</v>
+      </c>
+      <c r="B80">
+        <f>Sheet1!L94</f>
+        <v>14.374200000000002</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="str">
+        <f>Sheet1!A95</f>
+        <v>TMP_IS_30_C</v>
+      </c>
+      <c r="B81">
+        <f>Sheet1!L95</f>
+        <v>13.927400000000002</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" t="str">
+        <f>Sheet1!A96</f>
+        <v>TMP_IS_31_A</v>
+      </c>
+      <c r="B82">
+        <f>Sheet1!L96</f>
+        <v>14.2746</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" t="str">
+        <f>Sheet1!A97</f>
+        <v>TMP_IS_31_B</v>
+      </c>
+      <c r="B83">
+        <f>Sheet1!L97</f>
+        <v>14.958100000000002</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" t="str">
+        <f>Sheet1!A98</f>
+        <v>TMP_IS_31_C</v>
+      </c>
+      <c r="B84">
+        <f>Sheet1!L98</f>
+        <v>14.138000000000002</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" t="str">
+        <f>Sheet1!A99</f>
+        <v>TMP_IS_32_A</v>
+      </c>
+      <c r="B85">
+        <f>Sheet1!L99</f>
+        <v>13.162099999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" t="str">
+        <f>Sheet1!A100</f>
+        <v>TMP_IS_32_B</v>
+      </c>
+      <c r="B86">
+        <f>Sheet1!L100</f>
+        <v>13.6358</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" t="str">
+        <f>Sheet1!A101</f>
+        <v>TMP_IS_32_C</v>
+      </c>
+      <c r="B87">
+        <f>Sheet1!L101</f>
+        <v>12.812799999999999</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" t="str">
+        <f>Sheet1!A102</f>
+        <v>TMP_IS_33_A</v>
+      </c>
+      <c r="B88">
+        <f>Sheet1!L102</f>
+        <v>13.6983</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" t="str">
+        <f>Sheet1!A103</f>
+        <v>TMP_IS_33_B</v>
+      </c>
+      <c r="B89">
+        <f>Sheet1!L103</f>
+        <v>13.2363</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" t="str">
+        <f>Sheet1!A104</f>
+        <v>TMP_IS_33_C</v>
+      </c>
+      <c r="B90">
+        <f>Sheet1!L104</f>
+        <v>13.648099999999996</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" t="str">
+        <f>Sheet1!A105</f>
+        <v>TMP_IS_34_A</v>
+      </c>
+      <c r="B91">
+        <f>Sheet1!L105</f>
+        <v>13.887899999999998</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" t="str">
+        <f>Sheet1!A106</f>
+        <v>TMP_IS_34_B</v>
+      </c>
+      <c r="B92">
+        <f>Sheet1!L106</f>
+        <v>13.7118</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" t="str">
+        <f>Sheet1!A107</f>
+        <v>TMP_IS_34_C</v>
+      </c>
+      <c r="B93">
+        <f>Sheet1!L107</f>
+        <v>13.345100000000002</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" t="str">
+        <f>Sheet1!A108</f>
+        <v>TMP_IS_35_A</v>
+      </c>
+      <c r="B94">
+        <f>Sheet1!L108</f>
+        <v>13.650099999999998</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" t="str">
+        <f>Sheet1!A109</f>
+        <v>TMP_IS_35_B</v>
+      </c>
+      <c r="B95">
+        <f>Sheet1!L109</f>
+        <v>13.497900000000001</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" t="str">
+        <f>Sheet1!A110</f>
+        <v>TMP_IS_35_C</v>
+      </c>
+      <c r="B96">
+        <f>Sheet1!L110</f>
+        <v>14.121300000000005</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" t="str">
+        <f>Sheet1!A111</f>
+        <v>TMP_IS_36_A</v>
+      </c>
+      <c r="B97">
+        <f>Sheet1!L111</f>
+        <v>7.4527999999999999</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" t="str">
+        <f>Sheet1!A114</f>
+        <v>TMP_IS_37_A</v>
+      </c>
+      <c r="B98">
+        <f>Sheet1!L114</f>
+        <v>13.913199999999996</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" t="str">
+        <f>Sheet1!A115</f>
+        <v>TMP_IS_37_B</v>
+      </c>
+      <c r="B99">
+        <f>Sheet1!L115</f>
+        <v>14.331900000000005</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" t="str">
+        <f>Sheet1!A116</f>
+        <v>TMP_IS_37_C</v>
+      </c>
+      <c r="B100">
+        <f>Sheet1!L116</f>
+        <v>14.045900000000003</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" t="str">
+        <f>Sheet1!A117</f>
+        <v>TMP_IS_38_A</v>
+      </c>
+      <c r="B101">
+        <f>Sheet1!L117</f>
+        <v>14.383699999999997</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" t="str">
+        <f>Sheet1!A118</f>
+        <v>TMP_IS_38_B</v>
+      </c>
+      <c r="B102">
+        <f>Sheet1!L118</f>
+        <v>14.272500000000001</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" t="str">
+        <f>Sheet1!A119</f>
+        <v>TMP_IS_38_C</v>
+      </c>
+      <c r="B103">
+        <f>Sheet1!L119</f>
+        <v>15.291299999999996</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" t="str">
+        <f>Sheet1!A120</f>
+        <v>TMP_IS_39_A</v>
+      </c>
+      <c r="B104">
+        <f>Sheet1!L120</f>
+        <v>13.559700000000003</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" t="str">
+        <f>Sheet1!A121</f>
+        <v>TMP_IS_39_B</v>
+      </c>
+      <c r="B105">
+        <f>Sheet1!L121</f>
+        <v>14.758099999999999</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" t="str">
+        <f>Sheet1!A122</f>
+        <v>TMP_IS_39_C</v>
+      </c>
+      <c r="B106">
+        <f>Sheet1!L122</f>
+        <v>14.159300000000002</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" t="str">
+        <f>Sheet1!A123</f>
+        <v>TMP_IS_40_A</v>
+      </c>
+      <c r="B107">
+        <f>Sheet1!L123</f>
+        <v>12.891099999999998</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" t="str">
+        <f>Sheet1!A124</f>
+        <v>TMP_IS_40_B</v>
+      </c>
+      <c r="B108">
+        <f>Sheet1!L124</f>
+        <v>13.272299999999998</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" t="str">
+        <f>Sheet1!A125</f>
+        <v>TMP_IS_40_C</v>
+      </c>
+      <c r="B109">
+        <f>Sheet1!L125</f>
+        <v>12.670000000000002</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" t="str">
+        <f>Sheet1!A126</f>
+        <v>TMP_IS_41_A</v>
+      </c>
+      <c r="B110">
+        <f>Sheet1!L126</f>
+        <v>13.734500000000004</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" t="str">
+        <f>Sheet1!A127</f>
+        <v>TMP_IS_41_B</v>
+      </c>
+      <c r="B111">
+        <f>Sheet1!L127</f>
+        <v>13.355200000000004</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" t="str">
+        <f>Sheet1!A128</f>
+        <v>TMP_IS_41_C</v>
+      </c>
+      <c r="B112">
+        <f>Sheet1!L128</f>
+        <v>13.8154</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" t="str">
+        <f>Sheet1!A129</f>
+        <v>TMP_IS_42_A</v>
+      </c>
+      <c r="B113">
+        <f>Sheet1!L129</f>
+        <v>13.0717</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" t="str">
+        <f>Sheet1!A130</f>
+        <v>TMP_IS_42_B</v>
+      </c>
+      <c r="B114">
+        <f>Sheet1!L130</f>
+        <v>13.9633</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" t="str">
+        <f>Sheet1!A131</f>
+        <v>TMP_IS_42_C</v>
+      </c>
+      <c r="B115">
+        <f>Sheet1!L131</f>
+        <v>13.4436</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>